<commit_message>
Import excel tinggal validasi
</commit_message>
<xml_diff>
--- a/public/DataGsmMaster/users.xlsx
+++ b/public/DataGsmMaster/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C970406C-1560-45A1-88B7-D3CD2C6589C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E64BFE-34B3-4BE4-9655-D384007113B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Active</t>
   </si>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B1" sqref="B1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,33 +407,59 @@
     <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="B1" s="1">
         <v>1223</v>
       </c>
-      <c r="D1">
+      <c r="C1">
         <v>1</v>
       </c>
+      <c r="D1" s="1">
+        <v>2121233</v>
+      </c>
       <c r="E1" s="1">
-        <v>2121233</v>
+        <v>122132</v>
       </c>
       <c r="F1" s="1">
-        <v>122132</v>
+        <v>2121</v>
       </c>
       <c r="G1" s="1">
-        <v>2121</v>
-      </c>
-      <c r="H1" s="1">
-        <v>21213</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="2" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1223</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2121233</v>
+      </c>
+      <c r="E2" s="1">
+        <v>122132</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2121</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Filter tahun dan bulan
</commit_message>
<xml_diff>
--- a/public/DataGsmMaster/users.xlsx
+++ b/public/DataGsmMaster/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E64BFE-34B3-4BE4-9655-D384007113B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B9B2D2-EAFD-47C3-8965-55C45C5162D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="4605" windowWidth="16200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>Active</t>
   </si>
   <si>
     <t>we</t>
+  </si>
+  <si>
+    <t>telkomsel</t>
+  </si>
+  <si>
+    <t>tes</t>
   </si>
 </sst>
 </file>
@@ -393,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +413,7 @@
     <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,16 +442,19 @@
       <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>1223</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
       <c r="D2" s="1">
         <v>2121233</v>
@@ -461,6 +470,9 @@
       </c>
       <c r="L2" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>